<commit_message>
Selenium testcase added and exported after run
</commit_message>
<xml_diff>
--- a/DecicionTables.xlsx
+++ b/DecicionTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Conestoga\Sem-2\Software Quality\Assignment4\Assignment #4 – Automation Functional Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B078277B-F9BC-4739-904C-FF5F1E5B1E6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79B0E9A-7C01-4A60-A337-0834D86F657D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,9 +222,6 @@
     <t>InsuranceQuote14_BoundaryExperience</t>
   </si>
   <si>
-    <t>InsuranceQuote14_ValidEmail</t>
-  </si>
-  <si>
     <t>1. Enter valid name, address, city, province, and postal code.
 2. Enter Age = 25, Experience = 3, Accidents = 4.
 3. Submit the quote request.</t>
@@ -268,23 +265,12 @@
   </si>
   <si>
     <t>1. Enter valid name, address, city, province, and postal code.
-2. Enter Age = 46, Experience = 30 (16-year difference).
-3. Submit the quote request.</t>
-  </si>
-  <si>
-    <t>1. Enter valid name, address, city, province, and postal code.
 2. Enter Age = 40, Experience = 10, Accidents = 5.
 3. Submit the quote request.</t>
   </si>
   <si>
     <t>1. Enter valid name, address, city, province, and postal code.
 2. Enter Age = 32, Experience = 2 (minimum), Accidents = 1.
-3. Submit the quote request.</t>
-  </si>
-  <si>
-    <t>1. Enter valid name, address, city, province, and postal code
-(e.g., John Doe, 123 Main St, Anytown, ON, L1N 1A1).
-2. Enter Age = 24, Experience = 3, Accidents = 0.
 3. Submit the quote request.</t>
   </si>
   <si>
@@ -294,18 +280,6 @@
 3. Submit the quote request.</t>
   </si>
   <si>
-    <t>1. Enter valid name, address, city, province, and postal code.
-2. Enter Age = 38, Experience = 7, Accidents = 0.
-3. Submit the quote request with different valid email variations 
-(e.g., [email address removed]).</t>
-  </si>
-  <si>
-    <t>1. Enter valid name, address, city, province, and postal code.
-2. Enter Age = 30, Experience = 35 (invalid - experience cannot 
-be greater than age).
-3. Submit the quote request.</t>
-  </si>
-  <si>
     <t>System should display a message denying insurance.
 No annual rate should be displayed.</t>
   </si>
@@ -340,11 +314,6 @@
   <si>
     <t>System should display an error message indicating 
 invalid experience exceeding age.</t>
-  </si>
-  <si>
-    <t>System should process the quote request regardless 
-of minor email address variations as long as the 
-format is valid.</t>
   </si>
   <si>
     <t>System should display a message denying 
@@ -366,6 +335,34 @@
     <t xml:space="preserve">System should display a quote with insurance provided
 and annual rate should be $5500.
 </t>
+  </si>
+  <si>
+    <t>1. Enter valid name, address, city, province, and postal code.
+2. Enter Age = 24, Experience = 3, Accidents = 0.
+3. Submit the quote request.</t>
+  </si>
+  <si>
+    <t>1. Enter valid name, address, city, province, and postal code.
+2. Enter Age = 30, Experience = 35 (invalid - experience cannot 
+be greater than age),Accidents = 0.
+3. Submit the quote request.</t>
+  </si>
+  <si>
+    <t>1. Enter valid name, address, city, province, and postal code.
+2. Enter Age = 46, Experience = 30 (16-year difference),Accidents = 0.
+3. Submit the quote request.</t>
+  </si>
+  <si>
+    <t>1. Enter valid name, city, province, postal code.
+2. Enter Age = 45, Experience = 10, Accidents = 1.
+3. Omit street name from the address.
+4. Submit request.</t>
+  </si>
+  <si>
+    <t>InsuranceQuote15_InvalidAddress</t>
+  </si>
+  <si>
+    <t>System should display an error message indicating a missing street name in the address.</t>
   </si>
 </sst>
 </file>
@@ -514,12 +511,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,6 +530,12 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
@@ -550,26 +547,26 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <b/>
+      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -838,7 +835,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -883,22 +880,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
@@ -939,7 +920,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -952,6 +933,22 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -973,15 +970,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A53E07-6597-40C1-BA10-B17377E24704}" name="Table1" displayName="Table1" ref="B4:G14" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A53E07-6597-40C1-BA10-B17377E24704}" name="Table1" displayName="Table1" ref="B4:G14" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
   <autoFilter ref="B4:G14" xr:uid="{5EE8D5A2-67C6-4AD7-8F6E-7B2604A756B2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9146E7ED-E111-4C8B-8BD1-2B67AEDAD357}" name="S.No" dataDxfId="21" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="2" xr3:uid="{A1B5AD8E-E02C-4382-8E20-743B586DE688}" name="Age" dataDxfId="22" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="3" xr3:uid="{49855BF8-195B-4ACF-B771-E40231C23A67}" name="Driving Experience" dataDxfId="28" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="4" xr3:uid="{203539FE-49B6-46F1-8189-B1EEA0212765}" name="Number of Accidents" dataDxfId="27" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="5" xr3:uid="{53179AFD-0EC3-433B-ACF9-79EE1187D815}" name="Insurance Provided" dataDxfId="26" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="6" xr3:uid="{CEA26835-58B9-416C-8BFB-E3EB5F3B33D9}" name="Annual Rate" dataDxfId="25" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="1" xr3:uid="{9146E7ED-E111-4C8B-8BD1-2B67AEDAD357}" name="S.No" dataDxfId="26" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="2" xr3:uid="{A1B5AD8E-E02C-4382-8E20-743B586DE688}" name="Age" dataDxfId="25" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="3" xr3:uid="{49855BF8-195B-4ACF-B771-E40231C23A67}" name="Driving Experience" dataDxfId="24" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="4" xr3:uid="{203539FE-49B6-46F1-8189-B1EEA0212765}" name="Number of Accidents" dataDxfId="23" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="5" xr3:uid="{53179AFD-0EC3-433B-ACF9-79EE1187D815}" name="Insurance Provided" dataDxfId="22" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="6" xr3:uid="{CEA26835-58B9-416C-8BFB-E3EB5F3B33D9}" name="Annual Rate" dataDxfId="21" dataCellStyle="20% - Accent5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1017,13 +1014,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E4B073F6-9E65-415A-B302-6873255EC784}" name="Table7" displayName="Table7" ref="B44:E59" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E4B073F6-9E65-415A-B302-6873255EC784}" name="Table7" displayName="Table7" ref="B44:E59" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
   <autoFilter ref="B44:E59" xr:uid="{1C604BA8-B6BD-43E1-A712-8491DD3AF4DF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7A530962-17AE-4CAC-8236-5A5EC280520B}" name="TestID" dataDxfId="2" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="2" xr3:uid="{FD80B80E-2865-403F-9A66-C0A2CBF3E392}" name="Test Name" dataDxfId="5" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="3" xr3:uid="{DB834D23-832F-493B-AA0E-CA9D3BEC359C}" name="Test Steps" dataDxfId="0" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="4" xr3:uid="{B35D6AB4-FE66-4658-8BD9-E54EF38BA2C8}" name="Expected Outcome" dataDxfId="1" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="1" xr3:uid="{7A530962-17AE-4CAC-8236-5A5EC280520B}" name="TestID" dataDxfId="3" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="2" xr3:uid="{FD80B80E-2865-403F-9A66-C0A2CBF3E392}" name="Test Name" dataDxfId="2" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="3" xr3:uid="{DB834D23-832F-493B-AA0E-CA9D3BEC359C}" name="Test Steps" dataDxfId="1" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="4" xr3:uid="{B35D6AB4-FE66-4658-8BD9-E54EF38BA2C8}" name="Expected Outcome" dataDxfId="0" dataCellStyle="20% - Accent5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1294,21 +1291,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="54.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="11" customWidth="1"/>
     <col min="11" max="11" width="44.28515625" customWidth="1"/>
     <col min="12" max="12" width="60.85546875" customWidth="1"/>
     <col min="13" max="13" width="65.85546875" customWidth="1"/>
@@ -1322,7 +1319,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1345,7 +1342,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="7">
         <v>1</v>
       </c>
@@ -1365,8 +1362,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
       <c r="B6" s="7">
         <v>2</v>
       </c>
@@ -1386,8 +1383,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+    <row r="7" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -1407,8 +1404,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+    <row r="8" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -1428,8 +1425,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
       <c r="B9" s="7">
         <v>5</v>
       </c>
@@ -1450,7 +1447,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -1471,7 +1468,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="7">
         <v>7</v>
       </c>
@@ -1492,7 +1489,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="7">
         <v>8</v>
       </c>
@@ -1513,7 +1510,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="7">
         <v>9</v>
       </c>
@@ -1534,7 +1531,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="7">
         <v>10</v>
       </c>
@@ -1561,7 +1558,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1584,7 +1581,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="7">
         <v>1</v>
       </c>
@@ -1605,28 +1602,28 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11">
+      <c r="A21" s="17"/>
+      <c r="B21" s="9">
         <v>2</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="10">
         <v>0</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="7">
         <v>3</v>
       </c>
@@ -1647,28 +1644,28 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11">
+      <c r="A23" s="17"/>
+      <c r="B23" s="9">
         <v>4</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="7">
         <v>5</v>
       </c>
@@ -1689,28 +1686,28 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11">
+      <c r="A25" s="17"/>
+      <c r="B25" s="9">
         <v>6</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="7">
         <v>7</v>
       </c>
@@ -1731,28 +1728,28 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11">
+      <c r="A27" s="17"/>
+      <c r="B27" s="9">
         <v>8</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="7">
         <v>9</v>
       </c>
@@ -1773,23 +1770,23 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11">
+      <c r="A29" s="17"/>
+      <c r="B29" s="9">
         <v>10</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1800,7 +1797,7 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -1820,7 +1817,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="7">
         <v>1</v>
       </c>
@@ -1838,7 +1835,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="7">
         <v>2</v>
       </c>
@@ -1856,7 +1853,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="7">
         <v>3</v>
       </c>
@@ -1874,7 +1871,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="7">
         <v>4</v>
       </c>
@@ -1892,7 +1889,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="7">
         <v>5</v>
       </c>
@@ -1913,11 +1910,11 @@
       <c r="A42" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="13"/>
+      <c r="B42" s="11"/>
       <c r="D42"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="13"/>
+      <c r="B43" s="11"/>
       <c r="D43"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1934,214 +1931,214 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
+    <row r="45" spans="1:6" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="88.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B47" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="17" t="s">
+    </row>
+    <row r="49" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B51" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B52" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B53" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B55" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B56" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B58" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B59" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" s="15" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B46" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B52" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B53" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B54" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B55" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E55" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B56" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B57" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E58" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B59" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated/Modified Excel sheet and Added Docx file
</commit_message>
<xml_diff>
--- a/DecicionTables.xlsx
+++ b/DecicionTables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Conestoga\Sem-2\Software Quality\Assignment4\Assignment #4 – Automation Functional Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Conestoga\Sem-2\Software Quality\Assignment4\Assignment4_Automation Functional Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79B0E9A-7C01-4A60-A337-0834D86F657D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7640312C-A8F9-468A-9706-800A527D1BA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="78">
   <si>
     <t>S.No</t>
   </si>
@@ -123,61 +123,10 @@
     <t>Derived Test Cases</t>
   </si>
   <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>Test Name</t>
-  </si>
-  <si>
     <t>Test Steps</t>
   </si>
   <si>
     <t>Expected Outcome</t>
-  </si>
-  <si>
-    <t>IQTC-01</t>
-  </si>
-  <si>
-    <t>IQTC-02</t>
-  </si>
-  <si>
-    <t>IQTC-03</t>
-  </si>
-  <si>
-    <t>IQTC-04</t>
-  </si>
-  <si>
-    <t>IQTC-05</t>
-  </si>
-  <si>
-    <t>IQTC-06</t>
-  </si>
-  <si>
-    <t>IQTC-07</t>
-  </si>
-  <si>
-    <t>IQTC-08</t>
-  </si>
-  <si>
-    <t>IQTC-09</t>
-  </si>
-  <si>
-    <t>IQTC-10</t>
-  </si>
-  <si>
-    <t>IQTC-11</t>
-  </si>
-  <si>
-    <t>IQTC-12</t>
-  </si>
-  <si>
-    <t>IQTC-13</t>
-  </si>
-  <si>
-    <t>IQTC-14</t>
-  </si>
-  <si>
-    <t>IQTC-15</t>
   </si>
   <si>
     <t>InsuranceQuote01_ValidInput</t>
@@ -280,63 +229,6 @@
 3. Submit the quote request.</t>
   </si>
   <si>
-    <t>System should display a message denying insurance.
-No annual rate should be displayed.</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-an invalid phone number format</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-an invalid email address format.</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-an invalid postal code format.</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-a missing age.</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-missing information about the number of accidents.</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-missing information about the driving experience.</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-the minimum age requirement (16 years old).</t>
-  </si>
-  <si>
-    <t>System should display an error message indicating 
-invalid experience exceeding age.</t>
-  </si>
-  <si>
-    <t>System should display a message denying 
-insurance (denied for over 30 with 3 or more accidents).</t>
-  </si>
-  <si>
-    <t>System should process the quote request (valid 
-for someone over 30 with at least 2 years of experience).</t>
-  </si>
-  <si>
-    <t>System should process the quote(valid for someone 
-over 30 with at least 2 years of experience).</t>
-  </si>
-  <si>
-    <t>System should display a quote with insurance provided.
-Annual rate should be $4950 (29% reduction).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System should display a quote with insurance provided
-and annual rate should be $5500.
-</t>
-  </si>
-  <si>
     <t>1. Enter valid name, address, city, province, and postal code.
 2. Enter Age = 24, Experience = 3, Accidents = 0.
 3. Submit the quote request.</t>
@@ -362,14 +254,63 @@
     <t>InsuranceQuote15_InvalidAddress</t>
   </si>
   <si>
-    <t>System should display an error message indicating a missing street name in the address.</t>
+    <t>Verify that the system displays a quote with insurance provided and the annual rate should be $5500.</t>
+  </si>
+  <si>
+    <t>Verify that the System displays a message that states that insurance is refused.
+No annual rate should be displayed</t>
+  </si>
+  <si>
+    <t>Verify that the System displays a quote that includes the insurance provided.
+Annual rate should be $4950 (29% reduction).</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating an invalid phone number format.</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating an invalid email address format.</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating an invalid postal code format.</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating a missing age.</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating missing information about the number of accidents.</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating missing information about the driving experience.</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating the minimum age requirement (16 years old).</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating invalid experience exceeding age.</t>
+  </si>
+  <si>
+    <t>Verify that the system displays a message denying 
+insurance (denied for over 30 with 3 or more accidents).</t>
+  </si>
+  <si>
+    <t>Verify that the system displays an error message indicating a missing street name in the address.</t>
+  </si>
+  <si>
+    <t>Verify that the system processes the quote request (valid 
+for someone over 30 with at least 2 years of experience).</t>
+  </si>
+  <si>
+    <t>Verify that the system processes the quote(valid for someone over 30 with at least 2 years of experience).</t>
+  </si>
+  <si>
+    <t>Test ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,14 +329,6 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -484,30 +417,27 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
@@ -517,10 +447,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -530,10 +457,10 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,7 +472,7 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="28">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -554,12 +481,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -970,55 +891,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A53E07-6597-40C1-BA10-B17377E24704}" name="Table1" displayName="Table1" ref="B4:G14" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A53E07-6597-40C1-BA10-B17377E24704}" name="Table1" displayName="Table1" ref="B4:G14" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
   <autoFilter ref="B4:G14" xr:uid="{5EE8D5A2-67C6-4AD7-8F6E-7B2604A756B2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9146E7ED-E111-4C8B-8BD1-2B67AEDAD357}" name="S.No" dataDxfId="26" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="2" xr3:uid="{A1B5AD8E-E02C-4382-8E20-743B586DE688}" name="Age" dataDxfId="25" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="3" xr3:uid="{49855BF8-195B-4ACF-B771-E40231C23A67}" name="Driving Experience" dataDxfId="24" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="4" xr3:uid="{203539FE-49B6-46F1-8189-B1EEA0212765}" name="Number of Accidents" dataDxfId="23" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="5" xr3:uid="{53179AFD-0EC3-433B-ACF9-79EE1187D815}" name="Insurance Provided" dataDxfId="22" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="6" xr3:uid="{CEA26835-58B9-416C-8BFB-E3EB5F3B33D9}" name="Annual Rate" dataDxfId="21" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="1" xr3:uid="{9146E7ED-E111-4C8B-8BD1-2B67AEDAD357}" name="S.No" dataDxfId="25" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="2" xr3:uid="{A1B5AD8E-E02C-4382-8E20-743B586DE688}" name="Age" dataDxfId="24" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="3" xr3:uid="{49855BF8-195B-4ACF-B771-E40231C23A67}" name="Driving Experience" dataDxfId="23" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="4" xr3:uid="{203539FE-49B6-46F1-8189-B1EEA0212765}" name="Number of Accidents" dataDxfId="22" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="5" xr3:uid="{53179AFD-0EC3-433B-ACF9-79EE1187D815}" name="Insurance Provided" dataDxfId="21" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="6" xr3:uid="{CEA26835-58B9-416C-8BFB-E3EB5F3B33D9}" name="Annual Rate" dataDxfId="20" dataCellStyle="20% - Accent5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77555A9E-5C8C-46DD-9C2D-C611EDBE41EB}" name="Table13" displayName="Table13" ref="B19:G29" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77555A9E-5C8C-46DD-9C2D-C611EDBE41EB}" name="Table13" displayName="Table13" ref="B19:G29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
   <autoFilter ref="B19:G29" xr:uid="{6327ABC0-F307-405A-B695-79513F2E7BFB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5DB5652F-83FE-487A-8559-5665BB769517}" name="S.No" dataDxfId="18" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="2" xr3:uid="{1BFA1520-6641-4C07-8977-38558F475082}" name="Age" dataDxfId="17" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="3" xr3:uid="{546F6B8B-BE62-49F1-BA80-4C9E0FB6F2D0}" name="Driving Experience" dataDxfId="16" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="4" xr3:uid="{0BA1270F-51BC-4D0F-AEE1-12C5D333CC32}" name="Number of Accidents" dataDxfId="15" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="5" xr3:uid="{8CF9812C-B491-4D89-98D8-C49F1646BD97}" name="Insurance Provided" dataDxfId="14" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="6" xr3:uid="{6CE77B82-57AE-420D-8C8C-F6A76D584C40}" name="Annual Rate" dataDxfId="13" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="1" xr3:uid="{5DB5652F-83FE-487A-8559-5665BB769517}" name="S.No" dataDxfId="17" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="2" xr3:uid="{1BFA1520-6641-4C07-8977-38558F475082}" name="Age" dataDxfId="16" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="3" xr3:uid="{546F6B8B-BE62-49F1-BA80-4C9E0FB6F2D0}" name="Driving Experience" dataDxfId="15" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="4" xr3:uid="{0BA1270F-51BC-4D0F-AEE1-12C5D333CC32}" name="Number of Accidents" dataDxfId="14" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="5" xr3:uid="{8CF9812C-B491-4D89-98D8-C49F1646BD97}" name="Insurance Provided" dataDxfId="13" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="6" xr3:uid="{6CE77B82-57AE-420D-8C8C-F6A76D584C40}" name="Annual Rate" dataDxfId="12" dataCellStyle="20% - Accent5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4DF98CC5-6A16-456A-9E31-292845666B62}" name="Table134" displayName="Table134" ref="B34:F39" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4DF98CC5-6A16-456A-9E31-292845666B62}" name="Table134" displayName="Table134" ref="B34:F39" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
   <autoFilter ref="B34:F39" xr:uid="{85ACC138-D07E-431F-89C5-DEE68437E041}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E456DCFA-36F3-4820-A480-C80E6C4C350A}" name="S.No" dataDxfId="10" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="2" xr3:uid="{7FB7329E-5456-479A-AAA9-114DA65B8A86}" name="Age&gt;=30" dataDxfId="9" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="3" xr3:uid="{0E4BFED4-15C6-4A33-800A-A8BEDBC0C9CD}" name="Driving Experience" dataDxfId="8" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="4" xr3:uid="{8A8A6467-C2DD-4EE8-B762-81FFB32DA97F}" name="Insurance Provided" dataDxfId="7" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="5" xr3:uid="{16388865-26E3-4529-9C2E-CA5C38A67762}" name="Annual Rate" dataDxfId="6" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="1" xr3:uid="{E456DCFA-36F3-4820-A480-C80E6C4C350A}" name="S.No" dataDxfId="9" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="2" xr3:uid="{7FB7329E-5456-479A-AAA9-114DA65B8A86}" name="Age&gt;=30" dataDxfId="8" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="3" xr3:uid="{0E4BFED4-15C6-4A33-800A-A8BEDBC0C9CD}" name="Driving Experience" dataDxfId="7" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="4" xr3:uid="{8A8A6467-C2DD-4EE8-B762-81FFB32DA97F}" name="Insurance Provided" dataDxfId="6" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="5" xr3:uid="{16388865-26E3-4529-9C2E-CA5C38A67762}" name="Annual Rate" dataDxfId="5" dataCellStyle="20% - Accent5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E4B073F6-9E65-415A-B302-6873255EC784}" name="Table7" displayName="Table7" ref="B44:E59" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
-  <autoFilter ref="B44:E59" xr:uid="{1C604BA8-B6BD-43E1-A712-8491DD3AF4DF}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7A530962-17AE-4CAC-8236-5A5EC280520B}" name="TestID" dataDxfId="3" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="2" xr3:uid="{FD80B80E-2865-403F-9A66-C0A2CBF3E392}" name="Test Name" dataDxfId="2" dataCellStyle="20% - Accent5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E4B073F6-9E65-415A-B302-6873255EC784}" name="Table7" displayName="Table7" ref="C44:E59" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowCellStyle="Accent5" dataCellStyle="20% - Accent5">
+  <autoFilter ref="C44:E59" xr:uid="{1C604BA8-B6BD-43E1-A712-8491DD3AF4DF}"/>
+  <tableColumns count="3">
+    <tableColumn id="2" xr3:uid="{FD80B80E-2865-403F-9A66-C0A2CBF3E392}" name="Test ID" dataDxfId="2" dataCellStyle="20% - Accent5"/>
     <tableColumn id="3" xr3:uid="{DB834D23-832F-493B-AA0E-CA9D3BEC359C}" name="Test Steps" dataDxfId="1" dataCellStyle="20% - Accent5"/>
     <tableColumn id="4" xr3:uid="{B35D6AB4-FE66-4658-8BD9-E54EF38BA2C8}" name="Expected Outcome" dataDxfId="0" dataCellStyle="20% - Accent5"/>
   </tableColumns>
@@ -1289,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J59"/>
+  <dimension ref="A2:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1225,7 @@
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="10" customWidth="1"/>
     <col min="11" max="11" width="44.28515625" customWidth="1"/>
     <col min="12" max="12" width="60.85546875" customWidth="1"/>
     <col min="13" max="13" width="65.85546875" customWidth="1"/>
@@ -1313,833 +1233,791 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="7">
+      <c r="A5" s="15"/>
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="7">
+      <c r="A6" s="15"/>
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="7">
+      <c r="A7" s="15"/>
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="7">
+      <c r="A8" s="15"/>
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="7">
+      <c r="A9" s="15"/>
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="7">
+      <c r="A10" s="15"/>
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="7">
+      <c r="A11" s="15"/>
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="7">
+      <c r="A12" s="15"/>
+      <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="7">
+      <c r="A13" s="15"/>
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="7">
+      <c r="A14" s="15"/>
+      <c r="B14" s="6">
         <v>10</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="7">
+      <c r="A20" s="15"/>
+      <c r="B20" s="6">
         <v>1</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>0</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="9">
+      <c r="A21" s="15"/>
+      <c r="B21" s="8">
         <v>2</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>0</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="7">
+      <c r="A22" s="15"/>
+      <c r="B22" s="6">
         <v>3</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="9">
+      <c r="A23" s="15"/>
+      <c r="B23" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="7">
+      <c r="A24" s="15"/>
+      <c r="B24" s="6">
         <v>5</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="9">
+      <c r="A25" s="15"/>
+      <c r="B25" s="8">
         <v>6</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="7">
+      <c r="A26" s="15"/>
+      <c r="B26" s="6">
         <v>7</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="9">
+      <c r="A27" s="15"/>
+      <c r="B27" s="8">
         <v>8</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="7">
+      <c r="A28" s="15"/>
+      <c r="B28" s="6">
         <v>9</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="9">
+      <c r="A29" s="15"/>
+      <c r="B29" s="8">
         <v>10</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="7">
+      <c r="A35" s="15"/>
+      <c r="B35" s="6">
         <v>1</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <v>0</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="7">
+      <c r="A36" s="15"/>
+      <c r="B36" s="6">
         <v>2</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="7">
+      <c r="A37" s="15"/>
+      <c r="B37" s="6">
         <v>3</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="7">
+      <c r="A38" s="15"/>
+      <c r="B38" s="6">
         <v>4</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="7">
+      <c r="A39" s="15"/>
+      <c r="B39" s="6">
         <v>5</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="11"/>
+      <c r="B42" s="10"/>
       <c r="D42"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
+      <c r="B43" s="10"/>
       <c r="D43"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:6" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="D45" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="88.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+      <c r="D46" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C47" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="D47" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="C48" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="C49" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="88.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="13" t="s">
+      <c r="E49" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="C50" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C51" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E46" s="15" t="s">
+      <c r="E51" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="C52" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C53" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C54" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="C55" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="C56" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C57" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C58" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C59" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B47" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B49" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B50" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B51" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B52" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B54" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B55" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B56" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B57" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B58" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B59" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>93</v>
-      </c>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D60"/>
+      <c r="E60" s="1"/>
+      <c r="J60"/>
+      <c r="K60" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>